<commit_message>
table 3 table 4 done (tobacco)
</commit_message>
<xml_diff>
--- a/HNSCC_survivalAnalysis_marginS_tobacco.xlsx
+++ b/HNSCC_survivalAnalysis_marginS_tobacco.xlsx
@@ -12,11 +12,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="124">
   <si>
     <t>Reported by Tex Li-Hsing Chi. 
 tex@gate.sinica.edu.tw 
-2019-08-03</t>
+2019-08-07</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
@@ -25,6 +25,9 @@
     <t>Table 2. The clinicopathological features of HNSCC cohort association with tobacco exposure (Chi square test)</t>
   </si>
   <si>
+    <t>Cutoff at 38.9%</t>
+  </si>
+  <si>
     <t>tobacco exposure</t>
   </si>
   <si>
@@ -61,280 +64,328 @@
     <t>Matthews</t>
   </si>
   <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Age at diagnosis</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Clinical T Status</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Clinical N Status</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Clinical M Status</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Clinical Stage</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Surgical Margin status</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>&lt;=65y</t>
+  </si>
+  <si>
+    <t>&gt;65y</t>
+  </si>
+  <si>
+    <t>T1+T2</t>
+  </si>
+  <si>
+    <t>T3+T4</t>
+  </si>
+  <si>
+    <t>N0</t>
+  </si>
+  <si>
+    <t>N1-3</t>
+  </si>
+  <si>
+    <t>M0</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>Stage I+II</t>
+  </si>
+  <si>
+    <t>Stage III+IV</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
+    <t>51</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>23.9</t>
+  </si>
+  <si>
+    <t>14.9</t>
+  </si>
+  <si>
+    <t>21.4</t>
+  </si>
+  <si>
+    <t>17.3</t>
+  </si>
+  <si>
+    <t>17.6</t>
+  </si>
+  <si>
+    <t>21.2</t>
+  </si>
+  <si>
+    <t>23.4</t>
+  </si>
+  <si>
+    <t>15.4</t>
+  </si>
+  <si>
+    <t>38.6</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>12.3</t>
+  </si>
+  <si>
+    <t>26.5</t>
+  </si>
+  <si>
+    <t>29.6</t>
+  </si>
+  <si>
+    <t>9.2</t>
+  </si>
+  <si>
+    <t>207</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>185</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>178</t>
+  </si>
+  <si>
+    <t>119</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>252</t>
+  </si>
+  <si>
+    <t>203</t>
+  </si>
+  <si>
+    <t>195</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>49.9</t>
+  </si>
+  <si>
+    <t>11.3</t>
+  </si>
+  <si>
+    <t>44.6</t>
+  </si>
+  <si>
+    <t>16.6</t>
+  </si>
+  <si>
+    <t>18.3</t>
+  </si>
+  <si>
+    <t>42.9</t>
+  </si>
+  <si>
+    <t>28.7</t>
+  </si>
+  <si>
+    <t>32.5</t>
+  </si>
+  <si>
+    <t>60.7</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>48.9</t>
+  </si>
+  <si>
+    <t>14.2</t>
+  </si>
+  <si>
+    <t>415</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>3e-04</t>
+  </si>
+  <si>
+    <t>0.0016</t>
+  </si>
+  <si>
+    <t>0.0088</t>
+  </si>
+  <si>
+    <t>0.0099</t>
+  </si>
+  <si>
+    <t>Table 3. Univariate/Multivariate Cox's proportional hazards regression analyses on OS time of tobacco exposure in  HNSCC</t>
+  </si>
+  <si>
+    <t>Univariate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	</t>
+  </si>
+  <si>
+    <t>Multivariate</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>CI95%(L)</t>
+  </si>
+  <si>
+    <t>CI95%(H)</t>
   </si>
   <si>
     <t>11</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>13</t>
   </si>
   <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>&lt;=65y</t>
-  </si>
-  <si>
-    <t>&gt;65y</t>
-  </si>
-  <si>
-    <t>T1+T2</t>
-  </si>
-  <si>
-    <t>T3+T4</t>
-  </si>
-  <si>
-    <t>N0</t>
-  </si>
-  <si>
-    <t>N1-3</t>
-  </si>
-  <si>
-    <t>M0</t>
-  </si>
-  <si>
-    <t>M1</t>
-  </si>
-  <si>
-    <t>Stage I+II</t>
-  </si>
-  <si>
-    <t>Stage III+IV</t>
-  </si>
-  <si>
-    <t>Negative</t>
-  </si>
-  <si>
-    <t>Positive</t>
-  </si>
-  <si>
-    <t>99</t>
-  </si>
-  <si>
-    <t>62</t>
-  </si>
-  <si>
-    <t>89</t>
-  </si>
-  <si>
-    <t>72</t>
-  </si>
-  <si>
-    <t>73</t>
-  </si>
-  <si>
-    <t>88</t>
-  </si>
-  <si>
-    <t>97</t>
-  </si>
-  <si>
-    <t>64</t>
-  </si>
-  <si>
-    <t>160</t>
-  </si>
-  <si>
-    <t>51</t>
-  </si>
-  <si>
-    <t>110</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>23.9</t>
-  </si>
-  <si>
-    <t>14.9</t>
-  </si>
-  <si>
-    <t>21.4</t>
-  </si>
-  <si>
-    <t>17.3</t>
-  </si>
-  <si>
-    <t>17.6</t>
-  </si>
-  <si>
-    <t>21.2</t>
-  </si>
-  <si>
-    <t>23.4</t>
-  </si>
-  <si>
-    <t>15.4</t>
-  </si>
-  <si>
-    <t>38.6</t>
-  </si>
-  <si>
-    <t>0.2</t>
-  </si>
-  <si>
-    <t>12.3</t>
-  </si>
-  <si>
-    <t>26.5</t>
-  </si>
-  <si>
-    <t>29.6</t>
-  </si>
-  <si>
-    <t>9.2</t>
-  </si>
-  <si>
-    <t>207</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>185</t>
-  </si>
-  <si>
-    <t>69</t>
-  </si>
-  <si>
-    <t>76</t>
-  </si>
-  <si>
-    <t>178</t>
-  </si>
-  <si>
-    <t>119</t>
-  </si>
-  <si>
-    <t>135</t>
-  </si>
-  <si>
-    <t>252</t>
-  </si>
-  <si>
-    <t>203</t>
-  </si>
-  <si>
-    <t>195</t>
-  </si>
-  <si>
-    <t>59</t>
-  </si>
-  <si>
-    <t>49.9</t>
-  </si>
-  <si>
-    <t>11.3</t>
-  </si>
-  <si>
-    <t>44.6</t>
-  </si>
-  <si>
-    <t>16.6</t>
-  </si>
-  <si>
-    <t>18.3</t>
-  </si>
-  <si>
-    <t>42.9</t>
-  </si>
-  <si>
-    <t>28.7</t>
-  </si>
-  <si>
-    <t>32.5</t>
-  </si>
-  <si>
-    <t>60.7</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>48.9</t>
-  </si>
-  <si>
-    <t>14.2</t>
-  </si>
-  <si>
-    <t>415</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>3e-04</t>
-  </si>
-  <si>
-    <t>0.0016</t>
-  </si>
-  <si>
-    <t>0.0088</t>
-  </si>
-  <si>
-    <t>0.0099</t>
-  </si>
-  <si>
-    <t>Table 3. Univariate/Multivariate Cox's proportional hazards regression analyses on OS time of tobacco exposure in  HNSCC</t>
-  </si>
-  <si>
-    <t>Univariate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	</t>
-  </si>
-  <si>
-    <t>Multivariate</t>
-  </si>
-  <si>
-    <t>HR</t>
-  </si>
-  <si>
-    <t>CI95%(L)</t>
-  </si>
-  <si>
-    <t>CI95%(H)</t>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>Tobacco Exposure</t>
+  </si>
+  <si>
+    <t>0.37</t>
+  </si>
+  <si>
+    <t>0.06</t>
+  </si>
+  <si>
+    <t>0.03</t>
+  </si>
+  <si>
+    <t>0.25</t>
+  </si>
+  <si>
+    <t>0.05</t>
+  </si>
+  <si>
+    <t>0.21</t>
+  </si>
+  <si>
+    <t>***</t>
+  </si>
+  <si>
+    <t>0.04</t>
+  </si>
+  <si>
+    <t>Kaplan-Meier survival estimate: Cutoff at 38.9%</t>
   </si>
 </sst>
 </file>
@@ -342,7 +393,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="60">
+  <fonts count="57">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -675,30 +726,12 @@
     </font>
     <font>
       <name val="Calibri"/>
-      <sz val="12.0"/>
+      <sz val="14.0"/>
       <color rgb="000000"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color rgb="000000"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color rgb="000000"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color rgb="000000"/>
-      <b val="true"/>
+      <i val="true"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -717,6 +750,17 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF"/>
         <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ADD8E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ADD8E6"/>
+        <bgColor rgb="ADD8E6"/>
       </patternFill>
     </fill>
   </fills>
@@ -754,7 +798,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="247">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
@@ -869,25 +913,160 @@
     <xf numFmtId="0" fontId="46" fillId="4" borderId="4" xfId="0" applyBorder="true" applyFont="true" applyFill="true">
       <alignment horizontal="center" wrapText="true"/>
     </xf>
+    <xf numFmtId="0" fontId="45" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="47" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="48" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="49" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="50" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="51" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="52" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="53" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="54" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="55" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="45" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="48" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="49" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="50" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="51" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="52" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="53" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="54" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="55" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="45" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="47" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="48" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="49" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="50" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="51" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="52" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="53" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="54" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="55" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="45" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="48" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="49" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="50" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="51" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="52" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="53" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="54" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="55" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="45" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="47" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="48" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="49" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="50" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="51" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="52" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="53" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="54" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="55" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="45" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="48" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="49" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="50" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="51" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="52" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="53" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="54" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="55" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="45" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="47" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="48" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="49" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="50" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="51" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="52" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="53" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="54" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="55" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="45" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="48" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="49" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="50" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="51" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="52" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="53" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="54" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="55" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="45" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="47" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="48" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="49" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="50" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="51" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="52" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="53" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="54" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="55" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="45" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="48" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="49" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="50" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="51" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="52" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="53" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="54" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="55" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="45" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="47" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="48" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="49" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="50" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="51" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="52" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="53" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="54" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="55" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="45" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="48" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="49" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="50" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="51" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="52" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="53" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="54" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="55" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="45" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="47" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="48" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="49" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="50" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="51" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="52" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="53" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="54" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="55" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="45" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="47" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="48" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="49" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="50" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="51" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="52" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="53" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="54" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="55" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="45" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="47" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="48" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="49" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="50" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="51" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="52" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="53" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="54" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="55" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" wrapText="true"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="justify" vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
 </styleSheet>
@@ -960,501 +1139,503 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10"/>
+      <c r="B10" t="s" s="25">
+        <v>3</v>
+      </c>
     </row>
     <row r="11">
       <c r="D11" t="s" s="34">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E11" t="s" s="35">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F11" t="s" s="36">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G11" t="s" s="37">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H11" t="s" s="38">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12">
       <c r="B12"/>
       <c r="C12" t="s" s="44">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s" s="44">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E12" t="s" s="44">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F12" t="s" s="44">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s" s="44">
         <v>10</v>
       </c>
-      <c r="G12" t="s" s="44">
-        <v>9</v>
-      </c>
       <c r="H12" t="s" s="44">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I12" t="s" s="44">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J12" t="s" s="44">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K12" t="s" s="44">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s" s="40">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s" s="45">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s" s="46">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E13" t="s" s="47">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F13" t="s" s="48">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G13" t="s" s="49">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H13" t="s" s="50">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I13" t="s" s="51">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J13" t="s" s="52">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="K13" t="s" s="53">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s" s="40">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s" s="45">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s" s="46">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s" s="47">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F14" t="s" s="48">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G14" t="s" s="49">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H14" t="s" s="50">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I14" t="s" s="51">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J14" t="s" s="52">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K14" t="s" s="53">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s" s="40">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s" s="45">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s" s="46">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E15" t="s" s="47">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F15" t="s" s="48">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G15" t="s" s="49">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H15" t="s" s="50">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I15" t="s" s="51">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="J15" t="s" s="52">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="K15" t="s" s="53">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s" s="40">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s" s="45">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s" s="46">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E16" t="s" s="47">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F16" t="s" s="48">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G16" t="s" s="49">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H16" t="s" s="50">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I16" t="s" s="51">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J16" t="s" s="52">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K16" t="s" s="53">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s" s="40">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s" s="45">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s" s="46">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E17" t="s" s="47">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F17" t="s" s="48">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G17" t="s" s="49">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H17" t="s" s="50">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I17" t="s" s="51">
+        <v>99</v>
+      </c>
+      <c r="J17" t="s" s="52">
+        <v>53</v>
+      </c>
+      <c r="K17" t="s" s="53">
         <v>97</v>
-      </c>
-      <c r="J17" t="s" s="52">
-        <v>15</v>
-      </c>
-      <c r="K17" t="s" s="53">
-        <v>95</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s" s="40">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s" s="45">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D18" t="s" s="46">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E18" t="s" s="47">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F18" t="s" s="48">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G18" t="s" s="49">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H18" t="s" s="50">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I18" t="s" s="51">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J18" t="s" s="52">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K18" t="s" s="53">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s" s="40">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s" s="45">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s" s="46">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E19" t="s" s="47">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F19" t="s" s="48">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G19" t="s" s="49">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H19" t="s" s="50">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I19" t="s" s="51">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="J19" t="s" s="52">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="K19" t="s" s="53">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s" s="40">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s" s="45">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D20" t="s" s="46">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E20" t="s" s="47">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F20" t="s" s="48">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G20" t="s" s="49">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H20" t="s" s="50">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I20" t="s" s="51">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J20" t="s" s="52">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K20" t="s" s="53">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s" s="40">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s" s="45">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D21" t="s" s="46">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E21" t="s" s="47">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F21" t="s" s="48">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G21" t="s" s="49">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H21" t="s" s="50">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I21" t="s" s="51">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="J21" t="s" s="52">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="K21" t="s" s="53">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s" s="40">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s" s="45">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D22" t="s" s="46">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="E22" t="s" s="47">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F22" t="s" s="48">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G22" t="s" s="49">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H22" t="s" s="50">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I22" t="s" s="51">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J22" t="s" s="52">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K22" t="s" s="53">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s" s="40">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s" s="45">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D23" t="s" s="46">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E23" t="s" s="47">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F23" t="s" s="48">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G23" t="s" s="49">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H23" t="s" s="50">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I23" t="s" s="51">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J23" t="s" s="52">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="K23" t="s" s="53">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="s" s="40">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s" s="45">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D24" t="s" s="46">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E24" t="s" s="47">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F24" t="s" s="48">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G24" t="s" s="49">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H24" t="s" s="50">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I24" t="s" s="51">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J24" t="s" s="52">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K24" t="s" s="53">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s" s="40">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s" s="45">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D25" t="s" s="46">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E25" t="s" s="47">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F25" t="s" s="48">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G25" t="s" s="49">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H25" t="s" s="50">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I25" t="s" s="51">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="J25" t="s" s="52">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="K25" t="s" s="53">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s" s="40">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s" s="45">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D26" t="s" s="46">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E26" t="s" s="47">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F26" t="s" s="48">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G26" t="s" s="49">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H26" t="s" s="50">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I26" t="s" s="51">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J26" t="s" s="52">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K26" t="s" s="53">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27">
@@ -1494,7 +1675,7 @@
     </row>
     <row r="34">
       <c r="B34" t="s" s="63">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35">
@@ -1504,129 +1685,481 @@
     </row>
     <row r="36">
       <c r="D36" t="s" s="72">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E36" t="s" s="73">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F36" t="s" s="74">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G36" t="s" s="75">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H36" t="s" s="76">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" s="92"/>
       <c r="C37" t="s" s="93">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D37" t="s" s="93">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E37" t="s" s="93">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F37" t="s" s="93">
+        <v>108</v>
+      </c>
+      <c r="G37" t="s" s="93">
+        <v>13</v>
+      </c>
+      <c r="H37" t="s" s="93">
         <v>106</v>
       </c>
-      <c r="G37" t="s" s="93">
-        <v>12</v>
-      </c>
-      <c r="H37" t="s" s="93">
-        <v>104</v>
-      </c>
       <c r="I37" t="s" s="93">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="J37" t="s" s="93">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="K37" t="s" s="93">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="s">
-        <v>1</v>
-      </c>
+      <c r="B38" t="s" s="94">
+        <v>53</v>
+      </c>
+      <c r="C38" t="s" s="95">
+        <v>30</v>
+      </c>
+      <c r="D38" t="n" s="96">
+        <v>1.0</v>
+      </c>
+      <c r="E38" s="97"/>
+      <c r="F38" s="98"/>
+      <c r="G38" t="s" s="99">
+        <v>5</v>
+      </c>
+      <c r="H38" t="n" s="100">
+        <v>1.0</v>
+      </c>
+      <c r="I38" s="101"/>
+      <c r="J38" s="102"/>
+      <c r="K38" s="103"/>
     </row>
     <row r="39">
-      <c r="A39" t="s">
-        <v>1</v>
+      <c r="B39" t="s" s="104">
+        <v>16</v>
+      </c>
+      <c r="C39" t="s" s="105">
+        <v>31</v>
+      </c>
+      <c r="D39" t="n" s="106">
+        <v>1.16</v>
+      </c>
+      <c r="E39" t="n" s="107">
+        <v>0.84</v>
+      </c>
+      <c r="F39" t="n" s="108">
+        <v>1.59</v>
+      </c>
+      <c r="G39" t="s" s="109">
+        <v>115</v>
+      </c>
+      <c r="H39" t="n" s="110">
+        <v>1.2</v>
+      </c>
+      <c r="I39" t="n" s="111">
+        <v>0.86</v>
+      </c>
+      <c r="J39" t="n" s="112">
+        <v>1.68</v>
+      </c>
+      <c r="K39" t="n" s="113">
+        <v>0.28</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="s">
-        <v>1</v>
-      </c>
+      <c r="B40" t="s" s="114">
+        <v>109</v>
+      </c>
+      <c r="C40" t="s" s="115">
+        <v>32</v>
+      </c>
+      <c r="D40" t="n" s="116">
+        <v>1.0</v>
+      </c>
+      <c r="E40" s="117"/>
+      <c r="F40" s="118"/>
+      <c r="G40" t="s" s="119">
+        <v>5</v>
+      </c>
+      <c r="H40" t="n" s="120">
+        <v>1.0</v>
+      </c>
+      <c r="I40" s="121"/>
+      <c r="J40" s="122"/>
+      <c r="K40" s="123"/>
     </row>
     <row r="41">
-      <c r="A41" t="s">
-        <v>1</v>
+      <c r="B41" t="s" s="124">
+        <v>18</v>
+      </c>
+      <c r="C41" t="s" s="125">
+        <v>33</v>
+      </c>
+      <c r="D41" t="n" s="126">
+        <v>1.33</v>
+      </c>
+      <c r="E41" t="n" s="127">
+        <v>0.99</v>
+      </c>
+      <c r="F41" t="n" s="128">
+        <v>1.78</v>
+      </c>
+      <c r="G41" t="s" s="129">
+        <v>116</v>
+      </c>
+      <c r="H41" t="n" s="130">
+        <v>1.39</v>
+      </c>
+      <c r="I41" t="n" s="131">
+        <v>1.02</v>
+      </c>
+      <c r="J41" t="n" s="132">
+        <v>1.89</v>
+      </c>
+      <c r="K41" t="n" s="133">
+        <v>0.03</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="s">
-        <v>1</v>
-      </c>
+      <c r="B42" t="s" s="134">
+        <v>27</v>
+      </c>
+      <c r="C42" t="s" s="135">
+        <v>34</v>
+      </c>
+      <c r="D42" t="n" s="136">
+        <v>1.0</v>
+      </c>
+      <c r="E42" s="137"/>
+      <c r="F42" s="138"/>
+      <c r="G42" t="s" s="139">
+        <v>5</v>
+      </c>
+      <c r="H42" t="n" s="140">
+        <v>1.0</v>
+      </c>
+      <c r="I42" s="141"/>
+      <c r="J42" s="142"/>
+      <c r="K42" s="143"/>
     </row>
     <row r="43">
-      <c r="A43" t="s">
-        <v>1</v>
+      <c r="B43" t="s" s="144">
+        <v>20</v>
+      </c>
+      <c r="C43" t="s" s="145">
+        <v>35</v>
+      </c>
+      <c r="D43" t="n" s="146">
+        <v>1.41</v>
+      </c>
+      <c r="E43" t="n" s="147">
+        <v>1.03</v>
+      </c>
+      <c r="F43" t="n" s="148">
+        <v>1.93</v>
+      </c>
+      <c r="G43" t="s" s="149">
+        <v>117</v>
+      </c>
+      <c r="H43" t="n" s="150">
+        <v>2.2</v>
+      </c>
+      <c r="I43" t="n" s="151">
+        <v>1.16</v>
+      </c>
+      <c r="J43" t="n" s="152">
+        <v>4.16</v>
+      </c>
+      <c r="K43" t="n" s="153">
+        <v>0.02</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="s">
-        <v>1</v>
-      </c>
+      <c r="B44" t="s" s="154">
+        <v>110</v>
+      </c>
+      <c r="C44" t="s" s="155">
+        <v>36</v>
+      </c>
+      <c r="D44" t="n" s="156">
+        <v>1.0</v>
+      </c>
+      <c r="E44" s="157"/>
+      <c r="F44" s="158"/>
+      <c r="G44" t="s" s="159">
+        <v>5</v>
+      </c>
+      <c r="H44" t="n" s="160">
+        <v>1.0</v>
+      </c>
+      <c r="I44" s="161"/>
+      <c r="J44" s="162"/>
+      <c r="K44" s="163"/>
     </row>
     <row r="45">
-      <c r="A45" t="s">
-        <v>1</v>
+      <c r="B45" t="s" s="164">
+        <v>22</v>
+      </c>
+      <c r="C45" t="s" s="165">
+        <v>37</v>
+      </c>
+      <c r="D45" t="n" s="166">
+        <v>1.19</v>
+      </c>
+      <c r="E45" t="n" s="167">
+        <v>0.89</v>
+      </c>
+      <c r="F45" t="n" s="168">
+        <v>1.58</v>
+      </c>
+      <c r="G45" t="s" s="169">
+        <v>118</v>
+      </c>
+      <c r="H45" t="n" s="170">
+        <v>1.24</v>
+      </c>
+      <c r="I45" t="n" s="171">
+        <v>0.87</v>
+      </c>
+      <c r="J45" t="n" s="172">
+        <v>1.77</v>
+      </c>
+      <c r="K45" t="n" s="173">
+        <v>0.23</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="s">
-        <v>1</v>
-      </c>
+      <c r="B46" t="s" s="174">
+        <v>29</v>
+      </c>
+      <c r="C46" t="s" s="175">
+        <v>38</v>
+      </c>
+      <c r="D46" t="n" s="176">
+        <v>1.0</v>
+      </c>
+      <c r="E46" s="177"/>
+      <c r="F46" s="178"/>
+      <c r="G46" t="s" s="179">
+        <v>5</v>
+      </c>
+      <c r="H46" t="n" s="180">
+        <v>1.0</v>
+      </c>
+      <c r="I46" s="181"/>
+      <c r="J46" s="182"/>
+      <c r="K46" s="183"/>
     </row>
     <row r="47">
-      <c r="A47" t="s">
-        <v>1</v>
+      <c r="B47" t="s" s="184">
+        <v>24</v>
+      </c>
+      <c r="C47" t="s" s="185">
+        <v>39</v>
+      </c>
+      <c r="D47" t="n" s="186">
+        <v>4.1</v>
+      </c>
+      <c r="E47" t="n" s="187">
+        <v>1.01</v>
+      </c>
+      <c r="F47" t="n" s="188">
+        <v>16.64</v>
+      </c>
+      <c r="G47" t="s" s="189">
+        <v>119</v>
+      </c>
+      <c r="H47" t="n" s="190">
+        <v>9.41</v>
+      </c>
+      <c r="I47" t="n" s="191">
+        <v>2.05</v>
+      </c>
+      <c r="J47" t="n" s="192">
+        <v>43.12</v>
+      </c>
+      <c r="K47" t="n" s="193">
+        <v>0.0</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="s">
-        <v>1</v>
-      </c>
+      <c r="B48" t="s" s="194">
+        <v>111</v>
+      </c>
+      <c r="C48" t="s" s="195">
+        <v>40</v>
+      </c>
+      <c r="D48" t="n" s="196">
+        <v>1.0</v>
+      </c>
+      <c r="E48" s="197"/>
+      <c r="F48" s="198"/>
+      <c r="G48" t="s" s="199">
+        <v>5</v>
+      </c>
+      <c r="H48" t="n" s="200">
+        <v>1.0</v>
+      </c>
+      <c r="I48" s="201"/>
+      <c r="J48" s="202"/>
+      <c r="K48" s="203"/>
     </row>
     <row r="49">
-      <c r="A49" t="s">
-        <v>1</v>
+      <c r="B49" t="s" s="204">
+        <v>26</v>
+      </c>
+      <c r="C49" t="s" s="205">
+        <v>41</v>
+      </c>
+      <c r="D49" t="n" s="206">
+        <v>1.25</v>
+      </c>
+      <c r="E49" t="n" s="207">
+        <v>0.88</v>
+      </c>
+      <c r="F49" t="n" s="208">
+        <v>1.76</v>
+      </c>
+      <c r="G49" t="s" s="209">
+        <v>120</v>
+      </c>
+      <c r="H49" t="n" s="210">
+        <v>0.5</v>
+      </c>
+      <c r="I49" t="n" s="211">
+        <v>0.24</v>
+      </c>
+      <c r="J49" t="n" s="212">
+        <v>1.08</v>
+      </c>
+      <c r="K49" t="n" s="213">
+        <v>0.08</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="s">
-        <v>1</v>
-      </c>
+      <c r="B50" t="s" s="214">
+        <v>112</v>
+      </c>
+      <c r="C50" t="s" s="215">
+        <v>42</v>
+      </c>
+      <c r="D50" t="n" s="216">
+        <v>1.0</v>
+      </c>
+      <c r="E50" s="217"/>
+      <c r="F50" s="218"/>
+      <c r="G50" t="s" s="219">
+        <v>5</v>
+      </c>
+      <c r="H50" t="n" s="220">
+        <v>1.0</v>
+      </c>
+      <c r="I50" s="221"/>
+      <c r="J50" s="222"/>
+      <c r="K50" s="223"/>
     </row>
     <row r="51">
-      <c r="A51" t="s">
-        <v>1</v>
+      <c r="B51" t="s" s="224">
+        <v>28</v>
+      </c>
+      <c r="C51" t="s" s="225">
+        <v>43</v>
+      </c>
+      <c r="D51" t="n" s="226">
+        <v>1.59</v>
+      </c>
+      <c r="E51" t="n" s="227">
+        <v>1.16</v>
+      </c>
+      <c r="F51" t="n" s="228">
+        <v>2.19</v>
+      </c>
+      <c r="G51" t="s" s="229">
+        <v>121</v>
+      </c>
+      <c r="H51" t="n" s="230">
+        <v>1.67</v>
+      </c>
+      <c r="I51" t="n" s="231">
+        <v>1.21</v>
+      </c>
+      <c r="J51" t="n" s="232">
+        <v>2.31</v>
+      </c>
+      <c r="K51" t="n" s="233">
+        <v>0.0</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="s">
-        <v>1</v>
-      </c>
+      <c r="B52" t="s" s="234">
+        <v>113</v>
+      </c>
+      <c r="C52" t="s" s="235">
+        <v>9</v>
+      </c>
+      <c r="D52" t="n" s="236">
+        <v>1.0</v>
+      </c>
+      <c r="E52" s="237"/>
+      <c r="F52" s="238"/>
+      <c r="G52" t="s" s="239">
+        <v>5</v>
+      </c>
+      <c r="H52" t="n" s="240">
+        <v>1.0</v>
+      </c>
+      <c r="I52" s="241"/>
+      <c r="J52" s="242"/>
+      <c r="K52" s="243"/>
     </row>
     <row r="53">
-      <c r="A53" t="s">
-        <v>1</v>
+      <c r="B53" t="s" s="78">
+        <v>114</v>
+      </c>
+      <c r="C53" t="s" s="83">
+        <v>11</v>
+      </c>
+      <c r="D53" t="n" s="84">
+        <v>1.36</v>
+      </c>
+      <c r="E53" t="n" s="85">
+        <v>1.01</v>
+      </c>
+      <c r="F53" t="n" s="86">
+        <v>1.84</v>
+      </c>
+      <c r="G53" t="s" s="87">
+        <v>122</v>
+      </c>
+      <c r="H53" t="n" s="88">
+        <v>1.45</v>
+      </c>
+      <c r="I53" t="n" s="89">
+        <v>1.05</v>
+      </c>
+      <c r="J53" t="n" s="90">
+        <v>2.0</v>
+      </c>
+      <c r="K53" t="n" s="91">
+        <v>0.02</v>
       </c>
     </row>
     <row r="54">
@@ -1675,7 +2208,9 @@
       </c>
     </row>
     <row r="63">
-      <c r="B63"/>
+      <c r="A63" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
@@ -1744,12 +2279,68 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="B84" t="s" s="246">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="B1:F4"/>
+    <mergeCell ref="B84:F87"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>